<commit_message>
retain data in elevated_risk for hhms and child
</commit_message>
<xml_diff>
--- a/codebook/var_names_v6.xlsx
+++ b/codebook/var_names_v6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/codebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396DEACB-A767-8640-8902-04B083F38B5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30BD7E8-4A63-4979-B51A-39283B6FB291}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="15140" activeTab="2" xr2:uid="{FA921AC7-407C-8C48-B120-0A746313EBE5}"/>
+    <workbookView xWindow="780" yWindow="765" windowWidth="21600" windowHeight="10800" xr2:uid="{FA921AC7-407C-8C48-B120-0A746313EBE5}"/>
   </bookViews>
   <sheets>
     <sheet name="survey_6" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="668">
   <si>
     <t>oldname</t>
   </si>
@@ -2034,6 +2034,12 @@
   </si>
   <si>
     <t xml:space="preserve">w8_namesexage </t>
+  </si>
+  <si>
+    <t>hhm_elevated_risk</t>
+  </si>
+  <si>
+    <t>q28a_scale_1</t>
   </si>
 </sst>
 </file>
@@ -2393,19 +2399,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D122FC6-3A1F-904F-82C9-4DACE54BFF1F}">
-  <dimension ref="A1:B306"/>
+  <dimension ref="A1:B307"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2413,7 +2419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2421,7 +2427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2429,7 +2435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2437,7 +2443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2445,7 +2451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2461,7 +2467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2469,7 +2475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2477,7 +2483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2485,7 +2491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2493,7 +2499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2501,7 +2507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2509,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2517,7 +2523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2525,12 +2531,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2538,7 +2544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2546,7 +2552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2554,7 +2560,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2562,7 +2568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2570,7 +2576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2578,7 +2584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2586,7 +2592,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -2594,7 +2600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -2602,7 +2608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2610,7 +2616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2618,7 +2624,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -2626,7 +2632,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -2634,7 +2640,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -2642,7 +2648,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2650,7 +2656,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -2658,7 +2664,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -2666,7 +2672,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2674,7 +2680,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -2682,7 +2688,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -2690,7 +2696,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2698,7 +2704,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -2706,7 +2712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -2714,7 +2720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -2722,7 +2728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -2730,7 +2736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -2738,7 +2744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2746,7 +2752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -2754,7 +2760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -2762,7 +2768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -2778,7 +2784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -2786,7 +2792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>64</v>
       </c>
@@ -2794,7 +2800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>65</v>
       </c>
@@ -2802,7 +2808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -2810,7 +2816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -2818,7 +2824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -2826,7 +2832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>69</v>
       </c>
@@ -2834,7 +2840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -2842,7 +2848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -2850,7 +2856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -2858,7 +2864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -2866,7 +2872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -2882,7 +2888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -2890,7 +2896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -2898,7 +2904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -2906,7 +2912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -2914,7 +2920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -2922,7 +2928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -2930,7 +2936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -2938,7 +2944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -2946,7 +2952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -2954,7 +2960,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>88</v>
       </c>
@@ -2970,7 +2976,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>90</v>
       </c>
@@ -2978,7 +2984,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>92</v>
       </c>
@@ -2986,7 +2992,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>94</v>
       </c>
@@ -2994,7 +3000,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>96</v>
       </c>
@@ -3002,7 +3008,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>98</v>
       </c>
@@ -3010,7 +3016,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>100</v>
       </c>
@@ -3018,1835 +3024,1843 @@
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>667</v>
+      </c>
+      <c r="B78" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>102</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>104</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>106</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>108</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>110</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>112</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>114</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>116</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>118</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>120</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>122</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>124</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>126</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>128</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>130</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>132</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>134</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>136</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>138</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>140</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B98" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>142</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>144</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>146</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>148</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>150</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>152</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>154</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>156</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>158</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B107" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>160</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>162</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B109" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>164</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>166</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>168</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>170</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>172</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>174</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>176</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>178</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B117" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>180</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B118" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>182</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B119" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>184</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B120" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>186</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B121" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>188</v>
       </c>
-      <c r="B121" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+      <c r="B122" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>189</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>191</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B124" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>193</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B125" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>195</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B126" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B127" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B128" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>201</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B129" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>203</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B130" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>205</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B131" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>207</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B132" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>209</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B133" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>211</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B134" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B135" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>215</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B136" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>217</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B137" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>219</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B138" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>220</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B139" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>222</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B140" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>224</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B141" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>226</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B142" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>228</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B143" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>230</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B144" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>232</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B145" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>234</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B146" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>236</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B147" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>238</v>
       </c>
-      <c r="B147" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="B148" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>239</v>
       </c>
-      <c r="B148" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="B149" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>240</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B150" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>242</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B151" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>244</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B152" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>246</v>
       </c>
-      <c r="B152" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+      <c r="B153" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>247</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B154" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>249</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B155" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>251</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B156" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>253</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B157" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>255</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B158" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>257</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B159" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>259</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B160" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>261</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B161" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>263</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B162" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>265</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B163" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>267</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B164" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>269</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B165" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>271</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B166" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>273</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B167" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>275</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B168" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>277</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B169" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>279</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B170" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>281</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B171" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>283</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B172" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>285</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B173" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>287</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B174" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" t="s">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>289</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B175" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>291</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B176" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>293</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B177" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>295</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B178" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>297</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B179" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>299</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B180" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>301</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B181" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>303</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B182" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>305</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B183" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>307</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B184" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>309</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B185" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A185" t="s">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>311</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B186" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A186" t="s">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>313</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B187" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>315</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B188" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>317</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B189" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>319</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B190" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>321</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B191" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A191" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>323</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B192" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A192" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>325</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B193" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" t="s">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>327</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B194" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A194" s="1" t="s">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B194" s="1" t="s">
+      <c r="B195" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A195" t="s">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
         <v>331</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B196" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
         <v>333</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B197" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" t="s">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>335</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B198" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" t="s">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>337</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B199" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A199" s="1" t="s">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B199" s="1" t="s">
+      <c r="B200" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A200" t="s">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>341</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B201" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A201" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>343</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B202" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A202" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
         <v>345</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B203" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>347</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B204" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A204" s="1" t="s">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="B204" s="1" t="s">
+      <c r="B205" s="1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A205" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>351</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B206" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A206" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>353</v>
       </c>
-      <c r="B206" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A207" t="s">
+      <c r="B207" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>354</v>
       </c>
-      <c r="B207" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
+      <c r="B208" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>355</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B209" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A209" t="s">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
         <v>357</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B210" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A210" t="s">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
         <v>359</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B211" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A211" t="s">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>361</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B212" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A212" t="s">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>363</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B213" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
         <v>365</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B214" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>367</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B215" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A215" t="s">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>369</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B216" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>371</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B217" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A217" t="s">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>373</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B218" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>375</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B219" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A219" t="s">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
         <v>377</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B220" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A220" t="s">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>379</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B221" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A221" t="s">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>381</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B222" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A222" t="s">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>383</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B223" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A223" t="s">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>385</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B224" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A224" t="s">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>387</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B225" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A225" t="s">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>389</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B226" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A226" t="s">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
         <v>391</v>
       </c>
-      <c r="B226" t="s">
+      <c r="B227" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A227" t="s">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>393</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B228" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A228" t="s">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
         <v>395</v>
       </c>
-      <c r="B228" t="s">
+      <c r="B229" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A229" t="s">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
         <v>397</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B230" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A230" t="s">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
         <v>399</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B231" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A231" t="s">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
         <v>401</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B232" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A232" t="s">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
         <v>403</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B233" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A233" t="s">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
         <v>405</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B234" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A234" t="s">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
         <v>407</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B235" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A235" t="s">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
         <v>409</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B236" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A236" t="s">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
         <v>410</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B237" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A237" t="s">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
         <v>411</v>
       </c>
-      <c r="B237" t="s">
+      <c r="B238" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A238" t="s">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
         <v>413</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B239" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A239" t="s">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
         <v>415</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B240" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A240" t="s">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
         <v>417</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B241" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A241" t="s">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
         <v>419</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B242" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A242" t="s">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
         <v>421</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B243" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A243" t="s">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
         <v>423</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B244" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A244" t="s">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
         <v>425</v>
       </c>
-      <c r="B244" t="s">
+      <c r="B245" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A245" t="s">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
         <v>426</v>
       </c>
-      <c r="B245" t="s">
+      <c r="B246" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A246" t="s">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
         <v>427</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B247" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A247" t="s">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
         <v>428</v>
       </c>
-      <c r="B247" t="s">
+      <c r="B248" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A248" t="s">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
         <v>430</v>
       </c>
-      <c r="B248" t="s">
+      <c r="B249" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A249" t="s">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
         <v>432</v>
       </c>
-      <c r="B249" t="s">
+      <c r="B250" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A250" t="s">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
         <v>434</v>
       </c>
-      <c r="B250" t="s">
+      <c r="B251" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A251" t="s">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
         <v>436</v>
       </c>
-      <c r="B251" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A252" t="s">
+      <c r="B252" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
         <v>437</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B253" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A253" t="s">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
         <v>438</v>
       </c>
-      <c r="B253" t="s">
+      <c r="B254" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A254" t="s">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
         <v>440</v>
       </c>
-      <c r="B254" t="s">
+      <c r="B255" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A255" t="s">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
         <v>442</v>
       </c>
-      <c r="B255" t="s">
+      <c r="B256" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A256" t="s">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
         <v>444</v>
       </c>
-      <c r="B256" t="s">
+      <c r="B257" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A257" t="s">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
         <v>446</v>
       </c>
-      <c r="B257" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A258" t="s">
+      <c r="B258" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
         <v>447</v>
       </c>
-      <c r="B258" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A259" t="s">
+      <c r="B259" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
         <v>448</v>
       </c>
-      <c r="B259" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A260" t="s">
+      <c r="B260" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
         <v>449</v>
       </c>
-      <c r="B260" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A261" t="s">
+      <c r="B261" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
         <v>450</v>
       </c>
-      <c r="B261" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A262" t="s">
+      <c r="B262" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
         <v>451</v>
       </c>
-      <c r="B262" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A263" t="s">
+      <c r="B263" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
         <v>452</v>
       </c>
-      <c r="B263" t="s">
+      <c r="B264" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A264" t="s">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
         <v>453</v>
       </c>
-      <c r="B264" t="s">
+      <c r="B265" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A265" t="s">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
         <v>455</v>
       </c>
-      <c r="B265" t="s">
+      <c r="B266" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A266" t="s">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
         <v>457</v>
       </c>
-      <c r="B266" t="s">
+      <c r="B267" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A267" t="s">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
         <v>459</v>
       </c>
-      <c r="B267" t="s">
+      <c r="B268" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A268" t="s">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
         <v>461</v>
       </c>
-      <c r="B268" t="s">
+      <c r="B269" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A269" t="s">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
         <v>463</v>
       </c>
-      <c r="B269" t="s">
+      <c r="B270" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A270" t="s">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
         <v>465</v>
       </c>
-      <c r="B270" t="s">
+      <c r="B271" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A271" t="s">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
         <v>467</v>
       </c>
-      <c r="B271" t="s">
+      <c r="B272" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A272" t="s">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
         <v>469</v>
       </c>
-      <c r="B272" t="s">
+      <c r="B273" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A273" t="s">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
         <v>471</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B274" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A274" t="s">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
         <v>473</v>
       </c>
-      <c r="B274" t="s">
+      <c r="B275" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A275" t="s">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
         <v>475</v>
       </c>
-      <c r="B275" t="s">
+      <c r="B276" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A276" t="s">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
         <v>477</v>
       </c>
-      <c r="B276" t="s">
+      <c r="B277" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A277" t="s">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
         <v>479</v>
       </c>
-      <c r="B277" t="s">
+      <c r="B278" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A278" t="s">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
         <v>481</v>
       </c>
-      <c r="B278" t="s">
+      <c r="B279" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A279" t="s">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
         <v>483</v>
       </c>
-      <c r="B279" t="s">
+      <c r="B280" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A280" t="s">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
         <v>485</v>
       </c>
-      <c r="B280" t="s">
+      <c r="B281" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A281" t="s">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
         <v>487</v>
       </c>
-      <c r="B281" t="s">
+      <c r="B282" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A282" t="s">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
         <v>489</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B283" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A283" t="s">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
         <v>491</v>
       </c>
-      <c r="B283" t="s">
+      <c r="B284" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A284" t="s">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
         <v>493</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B285" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A285" t="s">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
         <v>495</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B286" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A286" t="s">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
         <v>497</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B287" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A287" t="s">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
         <v>499</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B288" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A288" t="s">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
         <v>501</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B289" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A289" t="s">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
         <v>503</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B290" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A290" t="s">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
         <v>505</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B291" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A291" t="s">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
         <v>507</v>
       </c>
-      <c r="B291" t="s">
+      <c r="B292" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A292" t="s">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
         <v>509</v>
       </c>
-      <c r="B292" t="s">
+      <c r="B293" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A293" t="s">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
         <v>511</v>
       </c>
-      <c r="B293" t="s">
+      <c r="B294" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A294" t="s">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
         <v>513</v>
       </c>
-      <c r="B294" t="s">
+      <c r="B295" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A295" t="s">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
         <v>515</v>
       </c>
-      <c r="B295" t="s">
+      <c r="B296" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A296" t="s">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
         <v>517</v>
       </c>
-      <c r="B296" t="s">
+      <c r="B297" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A297" t="s">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
         <v>519</v>
       </c>
-      <c r="B297" t="s">
+      <c r="B298" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A298" t="s">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
         <v>521</v>
       </c>
-      <c r="B298" t="s">
+      <c r="B299" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A299" t="s">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
         <v>523</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B300" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A300" t="s">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
         <v>525</v>
       </c>
-      <c r="B300" t="s">
+      <c r="B301" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A301" t="s">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
         <v>527</v>
       </c>
-      <c r="B301" t="s">
+      <c r="B302" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A302" t="s">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
         <v>529</v>
       </c>
-      <c r="B302" t="s">
+      <c r="B303" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A303" t="s">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
         <v>531</v>
       </c>
-      <c r="B303" t="s">
+      <c r="B304" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A304" t="s">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
         <v>533</v>
       </c>
-      <c r="B304" t="s">
+      <c r="B305" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A305" t="s">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
         <v>535</v>
       </c>
-      <c r="B305" t="s">
+      <c r="B306" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A306" t="s">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
         <v>537</v>
       </c>
-      <c r="B306" t="s">
+      <c r="B307" t="s">
         <v>538</v>
       </c>
     </row>
@@ -4863,9 +4877,9 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -4879,7 +4893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>540</v>
       </c>
@@ -4893,7 +4907,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>540</v>
       </c>
@@ -4907,7 +4921,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>540</v>
       </c>
@@ -4921,7 +4935,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>540</v>
       </c>
@@ -4935,7 +4949,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>540</v>
       </c>
@@ -4949,7 +4963,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>540</v>
       </c>
@@ -4963,7 +4977,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>540</v>
       </c>
@@ -4986,608 +5000,608 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98B2732-17DD-EE4A-94E5-45B96B3F7E1F}">
   <dimension ref="A1:A120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A120"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>665</v>
       </c>

</xml_diff>